<commit_message>
fixed continuous with previous bug
</commit_message>
<xml_diff>
--- a/Demo/Aventis - Pile Installation Simple.xlsx
+++ b/Demo/Aventis - Pile Installation Simple.xlsx
@@ -5735,8 +5735,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2343359116c41cd6df5e9933b71ba69e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bf6b77a57d9afd5d212f0342177a31b" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f83516c0962013713c7b05e4bc5e59d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="752b74123ce8ce04e6dc2ca32a236890" ns2:_="" ns3:_="">
     <xsd:import namespace="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
     <xsd:import namespace="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
     <xsd:element name="properties">
@@ -5757,6 +5757,7 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5849,6 +5850,11 @@
     <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5967,22 +5973,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49D3CA32-04D7-4B3D-A609-9C852A843DB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
-    <ds:schemaRef ds:uri="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D8FFA3-65C9-43F9-8D4E-F7555189104B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
added shift patterns so Aventis can now input start and end times each day. Export excel has also been smarted up to include persistence stats for each each activity, plots have been added and some minor formatting
</commit_message>
<xml_diff>
--- a/Demo/Aventis - Pile Installation Simple.xlsx
+++ b/Demo/Aventis - Pile Installation Simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://odslco.sharepoint.com/sites/PROJECTS/Shared Documents/RND - Research and Development/P-RND-ODSL-44053 AVENTIS Development/Code Development 2/Aventis/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="8_{7A62FD1D-008F-4E41-AAF6-0A55466296EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B12CFD63-71C4-4541-99EA-C1CC3DAF51A4}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{7A62FD1D-008F-4E41-AAF6-0A55466296EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5C31A2-4764-0440-8633-17DBDD5B8DA6}"/>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="500" windowWidth="14440" windowHeight="16460" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31140" yWindow="500" windowWidth="32300" windowHeight="21100" tabRatio="751" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="237">
   <si>
     <t>Simulation Info</t>
   </si>
@@ -707,6 +707,54 @@
   </si>
   <si>
     <t>Enter filepath to Demo/Weather and Properties/Demp_Weather_data.p</t>
+  </si>
+  <si>
+    <t>Cable Crossings</t>
+  </si>
+  <si>
+    <t>FRAGNET: Cable Crossing</t>
+  </si>
+  <si>
+    <t>Activity 1</t>
+  </si>
+  <si>
+    <t>Activity 2</t>
+  </si>
+  <si>
+    <t>Activity 3</t>
+  </si>
+  <si>
+    <t>Activity 4</t>
+  </si>
+  <si>
+    <t>Location 1</t>
+  </si>
+  <si>
+    <t>Location 2</t>
+  </si>
+  <si>
+    <t>Wave Steepness</t>
+  </si>
+  <si>
+    <t>Hs * Tp**2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; </t>
+  </si>
+  <si>
+    <t>Site Wave Steepness 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Wave Steepness 2 </t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>10, 12</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1293,9 +1341,6 @@
     <xf numFmtId="164" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="25" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2197,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AC62"/>
+  <dimension ref="B1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2291,28 +2336,28 @@
       <c r="AC2" s="3"/>
     </row>
     <row r="3" spans="2:29" s="1" customFormat="1" ht="20">
-      <c r="B3" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="148"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="148"/>
-      <c r="P3" s="148"/>
-      <c r="Q3" s="148"/>
-      <c r="R3" s="148"/>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="149"/>
+      <c r="B3" s="146" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="147"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="147"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="147"/>
+      <c r="O3" s="147"/>
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
+      <c r="U3" s="148"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
@@ -2648,9 +2693,7 @@
       <c r="B14" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>128</v>
-      </c>
+      <c r="C14" s="56"/>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
@@ -2715,7 +2758,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="38">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
@@ -2748,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
@@ -3393,7 +3436,7 @@
     </row>
     <row r="37" spans="2:29" s="1" customFormat="1" ht="23" customHeight="1">
       <c r="B37" s="70" t="s">
-        <v>6</v>
+        <v>227</v>
       </c>
       <c r="C37" s="57" t="s">
         <v>220</v>
@@ -3425,26 +3468,30 @@
       <c r="AC37" s="3"/>
     </row>
     <row r="38" spans="2:29" s="1" customFormat="1" ht="23" customHeight="1">
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="81"/>
-      <c r="N38" s="81"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="81"/>
-      <c r="Q38" s="81"/>
-      <c r="R38" s="81"/>
-      <c r="S38" s="81"/>
-      <c r="T38" s="81"/>
-      <c r="U38" s="82"/>
+      <c r="B38" s="76" t="s">
+        <v>228</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D38" s="77"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="80"/>
+      <c r="Q38" s="80"/>
+      <c r="R38" s="80"/>
+      <c r="S38" s="80"/>
+      <c r="T38" s="80"/>
+      <c r="U38" s="81"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
@@ -3454,26 +3501,26 @@
       <c r="AC38" s="3"/>
     </row>
     <row r="39" spans="2:29" s="1" customFormat="1" ht="9" customHeight="1">
-      <c r="B39" s="83"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="86"/>
-      <c r="L39" s="86"/>
-      <c r="M39" s="86"/>
-      <c r="N39" s="86"/>
-      <c r="O39" s="86"/>
-      <c r="P39" s="86"/>
-      <c r="Q39" s="86"/>
-      <c r="R39" s="86"/>
-      <c r="S39" s="86"/>
-      <c r="T39" s="86"/>
-      <c r="U39" s="87"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="85"/>
+      <c r="P39" s="85"/>
+      <c r="Q39" s="85"/>
+      <c r="R39" s="85"/>
+      <c r="S39" s="85"/>
+      <c r="T39" s="85"/>
+      <c r="U39" s="86"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
@@ -3505,30 +3552,30 @@
       <c r="U40" s="30"/>
     </row>
     <row r="41" spans="2:29" s="1" customFormat="1" ht="46" customHeight="1">
-      <c r="B41" s="88" t="s">
+      <c r="B41" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="91" t="s">
+      <c r="C41" s="88"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="88"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="91"/>
-      <c r="L41" s="91"/>
-      <c r="M41" s="91"/>
-      <c r="N41" s="91"/>
-      <c r="O41" s="91"/>
-      <c r="P41" s="91"/>
-      <c r="Q41" s="91"/>
-      <c r="R41" s="91"/>
-      <c r="S41" s="91"/>
-      <c r="T41" s="91"/>
-      <c r="U41" s="92"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="90"/>
+      <c r="N41" s="90"/>
+      <c r="O41" s="90"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90"/>
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="91"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
@@ -3538,64 +3585,64 @@
       <c r="AC41" s="3"/>
     </row>
     <row r="42" spans="2:29" s="1" customFormat="1" ht="73" customHeight="1">
-      <c r="B42" s="93" t="s">
+      <c r="B42" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="94" t="s">
+      <c r="C42" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="95" t="s">
+      <c r="D42" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="96" t="s">
+      <c r="E42" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="96" t="s">
+      <c r="F42" s="95" t="s">
         <v>215</v>
       </c>
-      <c r="G42" s="96" t="s">
+      <c r="G42" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="H42" s="96" t="s">
+      <c r="H42" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="I42" s="96" t="s">
+      <c r="I42" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="J42" s="97" t="s">
+      <c r="J42" s="96" t="s">
         <v>214</v>
       </c>
-      <c r="K42" s="97" t="s">
+      <c r="K42" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="L42" s="97" t="s">
+      <c r="L42" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="M42" s="97" t="s">
+      <c r="M42" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="N42" s="97" t="s">
+      <c r="N42" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="O42" s="97" t="s">
+      <c r="O42" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="P42" s="97" t="s">
+      <c r="P42" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="Q42" s="97" t="s">
+      <c r="Q42" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="R42" s="97" t="s">
+      <c r="R42" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="S42" s="97" t="s">
+      <c r="S42" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="T42" s="97" t="s">
+      <c r="T42" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="U42" s="98" t="s">
+      <c r="U42" s="97" t="s">
         <v>4</v>
       </c>
       <c r="W42" s="3"/>
@@ -3607,30 +3654,30 @@
       <c r="AC42" s="3"/>
     </row>
     <row r="43" spans="2:29" s="1" customFormat="1" ht="21" customHeight="1">
-      <c r="B43" s="99" t="s">
+      <c r="B43" s="98" t="s">
         <v>195</v>
       </c>
-      <c r="C43" s="100">
+      <c r="C43" s="99">
         <v>10</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="103"/>
-      <c r="G43" s="103"/>
-      <c r="H43" s="103"/>
-      <c r="I43" s="103"/>
-      <c r="J43" s="104"/>
-      <c r="K43" s="104"/>
-      <c r="L43" s="104"/>
-      <c r="M43" s="104"/>
-      <c r="N43" s="104"/>
-      <c r="O43" s="104"/>
-      <c r="P43" s="104"/>
-      <c r="Q43" s="104"/>
-      <c r="R43" s="104"/>
-      <c r="S43" s="104"/>
-      <c r="T43" s="104"/>
-      <c r="U43" s="105"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="102"/>
+      <c r="J43" s="103"/>
+      <c r="K43" s="103"/>
+      <c r="L43" s="103"/>
+      <c r="M43" s="103"/>
+      <c r="N43" s="103"/>
+      <c r="O43" s="103"/>
+      <c r="P43" s="103"/>
+      <c r="Q43" s="103"/>
+      <c r="R43" s="103"/>
+      <c r="S43" s="103"/>
+      <c r="T43" s="103"/>
+      <c r="U43" s="104"/>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
@@ -3639,27 +3686,31 @@
       <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
     </row>
-    <row r="44" spans="2:29" s="1" customFormat="1" ht="10" customHeight="1">
-      <c r="B44" s="106"/>
-      <c r="C44" s="107"/>
-      <c r="D44" s="107"/>
-      <c r="E44" s="107"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="107"/>
-      <c r="H44" s="107"/>
-      <c r="I44" s="107"/>
-      <c r="J44" s="108"/>
-      <c r="K44" s="108"/>
-      <c r="L44" s="108"/>
-      <c r="M44" s="108"/>
-      <c r="N44" s="108"/>
-      <c r="O44" s="108"/>
-      <c r="P44" s="108"/>
-      <c r="Q44" s="108"/>
-      <c r="R44" s="108"/>
-      <c r="S44" s="108"/>
-      <c r="T44" s="108"/>
-      <c r="U44" s="109"/>
+    <row r="44" spans="2:29" s="1" customFormat="1" ht="21" customHeight="1">
+      <c r="B44" s="98" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="99">
+        <v>7</v>
+      </c>
+      <c r="D44" s="100"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="102"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="102"/>
+      <c r="J44" s="103"/>
+      <c r="K44" s="103"/>
+      <c r="L44" s="103"/>
+      <c r="M44" s="103"/>
+      <c r="N44" s="103"/>
+      <c r="O44" s="103"/>
+      <c r="P44" s="103"/>
+      <c r="Q44" s="103"/>
+      <c r="R44" s="103"/>
+      <c r="S44" s="103"/>
+      <c r="T44" s="103"/>
+      <c r="U44" s="104"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
@@ -3668,29 +3719,27 @@
       <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
     </row>
-    <row r="45" spans="2:29" s="1" customFormat="1" ht="22" customHeight="1">
-      <c r="B45" s="110" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="111"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="107"/>
-      <c r="G45" s="107"/>
-      <c r="H45" s="107"/>
-      <c r="I45" s="107"/>
-      <c r="J45" s="108"/>
-      <c r="K45" s="108"/>
-      <c r="L45" s="108"/>
-      <c r="M45" s="108"/>
-      <c r="N45" s="108"/>
-      <c r="O45" s="108"/>
-      <c r="P45" s="108"/>
-      <c r="Q45" s="108"/>
-      <c r="R45" s="108"/>
-      <c r="S45" s="108"/>
-      <c r="T45" s="108"/>
-      <c r="U45" s="109"/>
+    <row r="45" spans="2:29" s="1" customFormat="1" ht="10" customHeight="1">
+      <c r="B45" s="105"/>
+      <c r="C45" s="106"/>
+      <c r="D45" s="106"/>
+      <c r="E45" s="106"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="106"/>
+      <c r="H45" s="106"/>
+      <c r="I45" s="106"/>
+      <c r="J45" s="107"/>
+      <c r="K45" s="107"/>
+      <c r="L45" s="107"/>
+      <c r="M45" s="107"/>
+      <c r="N45" s="107"/>
+      <c r="O45" s="107"/>
+      <c r="P45" s="107"/>
+      <c r="Q45" s="107"/>
+      <c r="R45" s="107"/>
+      <c r="S45" s="107"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="108"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
@@ -3699,29 +3748,29 @@
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
     </row>
-    <row r="46" spans="2:29" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="B46" s="114" t="s">
-        <v>204</v>
-      </c>
-      <c r="C46" s="115"/>
-      <c r="D46" s="115"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="115"/>
-      <c r="H46" s="115"/>
-      <c r="I46" s="115"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="115"/>
-      <c r="L46" s="115"/>
-      <c r="M46" s="115"/>
-      <c r="N46" s="115"/>
-      <c r="O46" s="115"/>
-      <c r="P46" s="115"/>
-      <c r="Q46" s="115"/>
-      <c r="R46" s="115"/>
-      <c r="S46" s="115"/>
-      <c r="T46" s="115"/>
-      <c r="U46" s="116"/>
+    <row r="46" spans="2:29" s="1" customFormat="1" ht="22" customHeight="1">
+      <c r="B46" s="109" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="110"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="106"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="106"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="107"/>
+      <c r="K46" s="107"/>
+      <c r="L46" s="107"/>
+      <c r="M46" s="107"/>
+      <c r="N46" s="107"/>
+      <c r="O46" s="107"/>
+      <c r="P46" s="107"/>
+      <c r="Q46" s="107"/>
+      <c r="R46" s="107"/>
+      <c r="S46" s="107"/>
+      <c r="T46" s="107"/>
+      <c r="U46" s="108"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
@@ -3730,43 +3779,29 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
     </row>
-    <row r="47" spans="2:29" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="B47" s="99" t="s">
-        <v>194</v>
-      </c>
-      <c r="C47" s="100">
-        <v>10</v>
-      </c>
-      <c r="D47" s="117">
-        <v>12</v>
-      </c>
-      <c r="E47" s="118">
-        <v>12</v>
-      </c>
-      <c r="F47" s="119"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="119"/>
-      <c r="I47" s="119" t="s">
-        <v>6</v>
-      </c>
-      <c r="J47" s="120"/>
-      <c r="K47" s="120" t="s">
-        <v>41</v>
-      </c>
-      <c r="L47" s="120" t="s">
-        <v>37</v>
-      </c>
-      <c r="M47" s="120">
-        <v>12</v>
-      </c>
-      <c r="N47" s="120"/>
-      <c r="O47" s="120"/>
-      <c r="P47" s="120"/>
-      <c r="Q47" s="120"/>
-      <c r="R47" s="120"/>
-      <c r="S47" s="120"/>
-      <c r="T47" s="120"/>
-      <c r="U47" s="121"/>
+    <row r="47" spans="2:29" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="B47" s="113" t="s">
+        <v>204</v>
+      </c>
+      <c r="C47" s="114"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="114"/>
+      <c r="H47" s="114"/>
+      <c r="I47" s="114"/>
+      <c r="J47" s="114"/>
+      <c r="K47" s="114"/>
+      <c r="L47" s="114"/>
+      <c r="M47" s="114"/>
+      <c r="N47" s="114"/>
+      <c r="O47" s="114"/>
+      <c r="P47" s="114"/>
+      <c r="Q47" s="114"/>
+      <c r="R47" s="114"/>
+      <c r="S47" s="114"/>
+      <c r="T47" s="114"/>
+      <c r="U47" s="115"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
@@ -3776,75 +3811,85 @@
       <c r="AC47" s="3"/>
     </row>
     <row r="48" spans="2:29" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="B48" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="100">
-        <v>1</v>
-      </c>
-      <c r="D48" s="118">
-        <v>100</v>
-      </c>
-      <c r="E48" s="118">
-        <v>4</v>
-      </c>
-      <c r="F48" s="119"/>
-      <c r="G48" s="119"/>
-      <c r="H48" s="119"/>
-      <c r="I48" s="119" t="s">
+      <c r="B48" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="99">
+        <v>10</v>
+      </c>
+      <c r="D48" s="116">
+        <v>12</v>
+      </c>
+      <c r="E48" s="117">
+        <v>12</v>
+      </c>
+      <c r="F48" s="118"/>
+      <c r="G48" s="118"/>
+      <c r="H48" s="118"/>
+      <c r="I48" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="120"/>
-      <c r="K48" s="120"/>
-      <c r="L48" s="120"/>
-      <c r="M48" s="120"/>
-      <c r="N48" s="120"/>
-      <c r="O48" s="120"/>
-      <c r="P48" s="120"/>
-      <c r="Q48" s="120"/>
-      <c r="R48" s="120"/>
-      <c r="S48" s="120"/>
-      <c r="T48" s="120"/>
-      <c r="U48" s="121"/>
+      <c r="J48" s="119"/>
+      <c r="K48" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="L48" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" s="119">
+        <v>12</v>
+      </c>
+      <c r="N48" s="119"/>
+      <c r="O48" s="119"/>
+      <c r="P48" s="119"/>
+      <c r="Q48" s="119"/>
+      <c r="R48" s="119"/>
+      <c r="S48" s="119"/>
+      <c r="T48" s="119"/>
+      <c r="U48" s="120"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
     </row>
     <row r="49" spans="2:29" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="B49" s="99" t="s">
-        <v>196</v>
-      </c>
-      <c r="C49" s="100">
-        <v>10</v>
-      </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="119"/>
-      <c r="G49" s="119"/>
-      <c r="H49" s="119"/>
-      <c r="I49" s="119"/>
-      <c r="J49" s="120"/>
-      <c r="K49" s="120"/>
-      <c r="L49" s="120"/>
-      <c r="M49" s="120"/>
-      <c r="N49" s="120"/>
-      <c r="O49" s="120"/>
-      <c r="P49" s="120"/>
-      <c r="Q49" s="120"/>
-      <c r="R49" s="120"/>
-      <c r="S49" s="120"/>
-      <c r="T49" s="120"/>
-      <c r="U49" s="121"/>
+      <c r="B49" s="98" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" s="99">
+        <v>1</v>
+      </c>
+      <c r="D49" s="117">
+        <v>100</v>
+      </c>
+      <c r="E49" s="117">
+        <v>4</v>
+      </c>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" s="119"/>
+      <c r="K49" s="119"/>
+      <c r="L49" s="119"/>
+      <c r="M49" s="119"/>
+      <c r="N49" s="119"/>
+      <c r="O49" s="119"/>
+      <c r="P49" s="119"/>
+      <c r="Q49" s="119"/>
+      <c r="R49" s="119"/>
+      <c r="S49" s="119"/>
+      <c r="T49" s="119"/>
+      <c r="U49" s="120"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z49" s="3"/>
       <c r="AA49" s="3"/>
@@ -3852,65 +3897,71 @@
       <c r="AC49" s="3"/>
     </row>
     <row r="50" spans="2:29" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="B50" s="99" t="s">
-        <v>190</v>
-      </c>
-      <c r="C50" s="100">
-        <v>1</v>
-      </c>
-      <c r="D50" s="118">
-        <v>100</v>
-      </c>
-      <c r="E50" s="118">
-        <v>4</v>
-      </c>
-      <c r="F50" s="119"/>
-      <c r="G50" s="119"/>
-      <c r="H50" s="119"/>
-      <c r="I50" s="119" t="s">
-        <v>6</v>
-      </c>
-      <c r="J50" s="120"/>
-      <c r="K50" s="120"/>
-      <c r="L50" s="120"/>
-      <c r="M50" s="120"/>
-      <c r="N50" s="120"/>
-      <c r="O50" s="120"/>
-      <c r="P50" s="120"/>
-      <c r="Q50" s="120"/>
-      <c r="R50" s="120"/>
-      <c r="S50" s="120"/>
-      <c r="T50" s="120"/>
-      <c r="U50" s="121"/>
+      <c r="B50" s="98" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="99">
+        <v>10</v>
+      </c>
+      <c r="D50" s="119"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="118"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="118"/>
+      <c r="I50" s="118"/>
+      <c r="J50" s="119"/>
+      <c r="K50" s="119"/>
+      <c r="L50" s="119"/>
+      <c r="M50" s="119"/>
+      <c r="N50" s="119"/>
+      <c r="O50" s="119"/>
+      <c r="P50" s="119"/>
+      <c r="Q50" s="119"/>
+      <c r="R50" s="119"/>
+      <c r="S50" s="119"/>
+      <c r="T50" s="119"/>
+      <c r="U50" s="120"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
+      <c r="Y50" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="Z50" s="3"/>
       <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
     </row>
-    <row r="51" spans="2:29" s="1" customFormat="1" ht="7" customHeight="1">
-      <c r="B51" s="122"/>
-      <c r="C51" s="123"/>
-      <c r="D51" s="124"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="126"/>
-      <c r="G51" s="126"/>
-      <c r="H51" s="126"/>
-      <c r="I51" s="126"/>
-      <c r="J51" s="127"/>
-      <c r="K51" s="127"/>
-      <c r="L51" s="127"/>
-      <c r="M51" s="127"/>
-      <c r="N51" s="127"/>
-      <c r="O51" s="127"/>
-      <c r="P51" s="127"/>
-      <c r="Q51" s="127"/>
-      <c r="R51" s="127"/>
-      <c r="S51" s="127"/>
-      <c r="T51" s="127"/>
-      <c r="U51" s="128"/>
+    <row r="51" spans="2:29" s="1" customFormat="1" ht="17" customHeight="1">
+      <c r="B51" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="99">
+        <v>1</v>
+      </c>
+      <c r="D51" s="117">
+        <v>100</v>
+      </c>
+      <c r="E51" s="117">
+        <v>4</v>
+      </c>
+      <c r="F51" s="118"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="118"/>
+      <c r="I51" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="119"/>
+      <c r="K51" s="119"/>
+      <c r="L51" s="119"/>
+      <c r="M51" s="119"/>
+      <c r="N51" s="119"/>
+      <c r="O51" s="119"/>
+      <c r="P51" s="119"/>
+      <c r="Q51" s="119"/>
+      <c r="R51" s="119"/>
+      <c r="S51" s="119"/>
+      <c r="T51" s="119"/>
+      <c r="U51" s="120"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
@@ -3919,29 +3970,27 @@
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
     </row>
-    <row r="52" spans="2:29" s="1" customFormat="1" ht="16" customHeight="1">
-      <c r="B52" s="114" t="s">
-        <v>203</v>
-      </c>
-      <c r="C52" s="129"/>
-      <c r="D52" s="129"/>
-      <c r="E52" s="129"/>
-      <c r="F52" s="129"/>
-      <c r="G52" s="129"/>
-      <c r="H52" s="129"/>
-      <c r="I52" s="129"/>
-      <c r="J52" s="129"/>
-      <c r="K52" s="129"/>
-      <c r="L52" s="129"/>
-      <c r="M52" s="129"/>
-      <c r="N52" s="129"/>
-      <c r="O52" s="129"/>
-      <c r="P52" s="129"/>
-      <c r="Q52" s="129"/>
-      <c r="R52" s="129"/>
-      <c r="S52" s="129"/>
-      <c r="T52" s="129"/>
-      <c r="U52" s="130"/>
+    <row r="52" spans="2:29" s="1" customFormat="1" ht="7" customHeight="1">
+      <c r="B52" s="121"/>
+      <c r="C52" s="122"/>
+      <c r="D52" s="123"/>
+      <c r="E52" s="124"/>
+      <c r="F52" s="125"/>
+      <c r="G52" s="125"/>
+      <c r="H52" s="125"/>
+      <c r="I52" s="125"/>
+      <c r="J52" s="126"/>
+      <c r="K52" s="126"/>
+      <c r="L52" s="126"/>
+      <c r="M52" s="126"/>
+      <c r="N52" s="126"/>
+      <c r="O52" s="126"/>
+      <c r="P52" s="126"/>
+      <c r="Q52" s="126"/>
+      <c r="R52" s="126"/>
+      <c r="S52" s="126"/>
+      <c r="T52" s="126"/>
+      <c r="U52" s="127"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
@@ -3950,452 +3999,738 @@
       <c r="AB52" s="3"/>
       <c r="AC52" s="3"/>
     </row>
-    <row r="53" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B53" s="131" t="s">
+    <row r="53" spans="2:29" s="1" customFormat="1" ht="16" customHeight="1">
+      <c r="B53" s="113" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="128"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="128"/>
+      <c r="F53" s="128"/>
+      <c r="G53" s="128"/>
+      <c r="H53" s="128"/>
+      <c r="I53" s="128"/>
+      <c r="J53" s="128"/>
+      <c r="K53" s="128"/>
+      <c r="L53" s="128"/>
+      <c r="M53" s="128"/>
+      <c r="N53" s="128"/>
+      <c r="O53" s="128"/>
+      <c r="P53" s="128"/>
+      <c r="Q53" s="128"/>
+      <c r="R53" s="128"/>
+      <c r="S53" s="128"/>
+      <c r="T53" s="128"/>
+      <c r="U53" s="129"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="3"/>
+      <c r="AC53" s="3"/>
+    </row>
+    <row r="54" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B54" s="130" t="s">
         <v>193</v>
       </c>
-      <c r="C53" s="100">
+      <c r="C54" s="99">
         <v>1</v>
       </c>
-      <c r="D53" s="118">
+      <c r="D54" s="117">
         <v>1</v>
       </c>
-      <c r="E53" s="118">
+      <c r="E54" s="117">
         <v>3</v>
       </c>
-      <c r="F53" s="119"/>
-      <c r="G53" s="119"/>
-      <c r="H53" s="119"/>
-      <c r="I53" s="119" t="s">
+      <c r="F54" s="118"/>
+      <c r="G54" s="118"/>
+      <c r="H54" s="118"/>
+      <c r="I54" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="J53" s="120"/>
-      <c r="K53" s="120" t="s">
+      <c r="J54" s="119"/>
+      <c r="K54" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="L53" s="120" t="s">
+      <c r="L54" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="M53" s="120">
+      <c r="M54" s="119">
         <v>2</v>
       </c>
-      <c r="N53" s="120"/>
-      <c r="O53" s="120" t="s">
+      <c r="N54" s="119"/>
+      <c r="O54" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="P53" s="120" t="s">
+      <c r="P54" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="Q53" s="120">
+      <c r="Q54" s="119">
         <v>14</v>
       </c>
-      <c r="R53" s="120"/>
-      <c r="S53" s="120"/>
-      <c r="T53" s="132"/>
-      <c r="U53" s="121"/>
-    </row>
-    <row r="54" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B54" s="133" t="s">
+      <c r="R54" s="119"/>
+      <c r="S54" s="119"/>
+      <c r="T54" s="131"/>
+      <c r="U54" s="120"/>
+    </row>
+    <row r="55" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B55" s="132" t="s">
         <v>197</v>
       </c>
-      <c r="C54" s="134">
+      <c r="C55" s="133">
         <v>1</v>
       </c>
-      <c r="D54" s="135">
+      <c r="D55" s="134">
         <v>1</v>
       </c>
-      <c r="E54" s="102">
+      <c r="E55" s="101">
         <v>9</v>
       </c>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="H54" s="136"/>
-      <c r="I54" s="136" t="s">
+      <c r="F55" s="135"/>
+      <c r="G55" s="135"/>
+      <c r="H55" s="135"/>
+      <c r="I55" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J54" s="104" t="s">
+      <c r="J55" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K54" s="104" t="s">
+      <c r="K55" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L54" s="104" t="s">
+      <c r="L55" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M54" s="104">
+      <c r="M55" s="103">
         <v>2</v>
       </c>
-      <c r="N54" s="104"/>
-      <c r="O54" s="104" t="s">
+      <c r="N55" s="103"/>
+      <c r="O55" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P54" s="104" t="s">
+      <c r="P55" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q54" s="104">
+      <c r="Q55" s="103">
         <v>6</v>
       </c>
-      <c r="R54" s="104"/>
-      <c r="S54" s="120" t="s">
+      <c r="R55" s="103"/>
+      <c r="S55" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="T54" s="104" t="s">
+      <c r="T55" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="U54" s="105">
+      <c r="U55" s="104">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B55" s="137" t="s">
+    <row r="56" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B56" s="136" t="s">
         <v>198</v>
       </c>
-      <c r="C55" s="134">
+      <c r="C56" s="133">
         <v>1</v>
       </c>
-      <c r="D55" s="135">
+      <c r="D56" s="134">
         <v>1.5</v>
       </c>
-      <c r="E55" s="102">
+      <c r="E56" s="101">
         <v>2</v>
       </c>
-      <c r="F55" s="136"/>
-      <c r="G55" s="136"/>
-      <c r="H55" s="136"/>
-      <c r="I55" s="136" t="s">
+      <c r="F56" s="135"/>
+      <c r="G56" s="135"/>
+      <c r="H56" s="135"/>
+      <c r="I56" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J55" s="104" t="s">
+      <c r="J56" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="104" t="s">
+      <c r="K56" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="104" t="s">
+      <c r="L56" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M55" s="104">
+      <c r="M56" s="103">
         <v>2</v>
       </c>
-      <c r="N55" s="104"/>
-      <c r="O55" s="104" t="s">
+      <c r="N56" s="103"/>
+      <c r="O56" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P55" s="104" t="s">
+      <c r="P56" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q55" s="104">
+      <c r="Q56" s="103">
         <v>6</v>
       </c>
-      <c r="R55" s="104"/>
-      <c r="S55" s="104"/>
-      <c r="T55" s="104"/>
-      <c r="U55" s="105"/>
-    </row>
-    <row r="56" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B56" s="133" t="s">
+      <c r="R56" s="103"/>
+      <c r="S56" s="103"/>
+      <c r="T56" s="103"/>
+      <c r="U56" s="104"/>
+    </row>
+    <row r="57" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B57" s="132" t="s">
         <v>199</v>
       </c>
-      <c r="C56" s="134">
+      <c r="C57" s="133">
         <v>1</v>
       </c>
-      <c r="D56" s="135">
+      <c r="D57" s="134">
         <v>2</v>
       </c>
-      <c r="E56" s="102">
+      <c r="E57" s="101">
         <v>2</v>
       </c>
-      <c r="F56" s="136"/>
-      <c r="G56" s="136"/>
-      <c r="H56" s="136"/>
-      <c r="I56" s="136" t="s">
+      <c r="F57" s="135"/>
+      <c r="G57" s="135"/>
+      <c r="H57" s="135"/>
+      <c r="I57" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J56" s="104" t="s">
+      <c r="J57" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K56" s="104" t="s">
+      <c r="K57" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L56" s="104" t="s">
+      <c r="L57" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M56" s="104">
+      <c r="M57" s="103">
         <v>2</v>
       </c>
-      <c r="N56" s="104"/>
-      <c r="O56" s="104" t="s">
+      <c r="N57" s="103"/>
+      <c r="O57" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P56" s="104" t="s">
+      <c r="P57" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q56" s="104">
+      <c r="Q57" s="103">
         <v>6</v>
       </c>
-      <c r="R56" s="104"/>
-      <c r="S56" s="104"/>
-      <c r="T56" s="104"/>
-      <c r="U56" s="105"/>
-    </row>
-    <row r="57" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B57" s="133" t="s">
+      <c r="R57" s="103"/>
+      <c r="S57" s="103"/>
+      <c r="T57" s="103"/>
+      <c r="U57" s="104"/>
+    </row>
+    <row r="58" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B58" s="132" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="134">
+      <c r="C58" s="133">
         <v>1</v>
       </c>
-      <c r="D57" s="135">
+      <c r="D58" s="134">
         <v>4</v>
       </c>
-      <c r="E57" s="102">
+      <c r="E58" s="101">
         <v>6</v>
       </c>
-      <c r="F57" s="136"/>
-      <c r="G57" s="136"/>
-      <c r="H57" s="136"/>
-      <c r="I57" s="136" t="s">
+      <c r="F58" s="135"/>
+      <c r="G58" s="135"/>
+      <c r="H58" s="135"/>
+      <c r="I58" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="104" t="s">
+      <c r="J58" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="104" t="s">
+      <c r="K58" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L57" s="104" t="s">
+      <c r="L58" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M57" s="104">
+      <c r="M58" s="103">
         <v>2</v>
       </c>
-      <c r="N57" s="104"/>
-      <c r="O57" s="104" t="s">
+      <c r="N58" s="103"/>
+      <c r="O58" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P57" s="104" t="s">
+      <c r="P58" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q57" s="104">
+      <c r="Q58" s="103">
         <v>6</v>
       </c>
-      <c r="R57" s="104"/>
-      <c r="S57" s="104"/>
-      <c r="T57" s="104"/>
-      <c r="U57" s="105"/>
-    </row>
-    <row r="58" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B58" s="133" t="s">
+      <c r="R58" s="103"/>
+      <c r="S58" s="103"/>
+      <c r="T58" s="103"/>
+      <c r="U58" s="104"/>
+    </row>
+    <row r="59" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B59" s="132" t="s">
         <v>201</v>
       </c>
-      <c r="C58" s="134">
+      <c r="C59" s="133">
         <v>1</v>
       </c>
-      <c r="D58" s="135">
+      <c r="D59" s="134">
         <v>4</v>
       </c>
-      <c r="E58" s="102">
+      <c r="E59" s="101">
         <v>6</v>
       </c>
-      <c r="F58" s="136"/>
-      <c r="G58" s="136"/>
-      <c r="H58" s="136"/>
-      <c r="I58" s="136" t="s">
+      <c r="F59" s="135"/>
+      <c r="G59" s="135"/>
+      <c r="H59" s="135"/>
+      <c r="I59" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J58" s="104" t="s">
+      <c r="J59" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K58" s="104" t="s">
+      <c r="K59" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L58" s="104" t="s">
+      <c r="L59" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M58" s="104">
+      <c r="M59" s="103">
         <v>2</v>
       </c>
-      <c r="N58" s="104"/>
-      <c r="O58" s="104" t="s">
+      <c r="N59" s="103"/>
+      <c r="O59" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P58" s="104" t="s">
+      <c r="P59" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q58" s="104">
+      <c r="Q59" s="103">
         <v>6</v>
       </c>
-      <c r="R58" s="104"/>
-      <c r="S58" s="104"/>
-      <c r="T58" s="104"/>
-      <c r="U58" s="105"/>
-    </row>
-    <row r="59" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B59" s="133" t="s">
+      <c r="R59" s="103"/>
+      <c r="S59" s="103"/>
+      <c r="T59" s="103"/>
+      <c r="U59" s="104"/>
+    </row>
+    <row r="60" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B60" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="C59" s="134">
+      <c r="C60" s="133">
         <v>1</v>
       </c>
-      <c r="D59" s="135">
+      <c r="D60" s="134">
         <v>4</v>
       </c>
-      <c r="E59" s="102">
+      <c r="E60" s="101">
         <v>6</v>
       </c>
-      <c r="F59" s="136"/>
-      <c r="G59" s="136"/>
-      <c r="H59" s="136"/>
-      <c r="I59" s="136" t="s">
+      <c r="F60" s="135"/>
+      <c r="G60" s="135"/>
+      <c r="H60" s="135"/>
+      <c r="I60" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="J59" s="104" t="s">
+      <c r="J60" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="K59" s="104" t="s">
+      <c r="K60" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L59" s="104" t="s">
+      <c r="L60" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M59" s="104">
+      <c r="M60" s="103">
         <v>2</v>
       </c>
-      <c r="N59" s="104"/>
-      <c r="O59" s="104" t="s">
+      <c r="N60" s="103"/>
+      <c r="O60" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P59" s="104" t="s">
+      <c r="P60" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q59" s="104">
+      <c r="Q60" s="103">
         <v>6</v>
       </c>
-      <c r="R59" s="104"/>
-      <c r="S59" s="104"/>
-      <c r="T59" s="104"/>
-      <c r="U59" s="105"/>
-    </row>
-    <row r="60" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B60" s="131" t="s">
+      <c r="R60" s="103"/>
+      <c r="S60" s="103"/>
+      <c r="T60" s="103"/>
+      <c r="U60" s="104"/>
+    </row>
+    <row r="61" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B61" s="130" t="s">
         <v>192</v>
       </c>
-      <c r="C60" s="100">
+      <c r="C61" s="99">
         <v>1</v>
       </c>
-      <c r="D60" s="118">
+      <c r="D61" s="117">
         <v>1</v>
       </c>
-      <c r="E60" s="118">
-        <f>D60</f>
+      <c r="E61" s="117">
+        <f>D61</f>
         <v>1</v>
       </c>
-      <c r="F60" s="119"/>
-      <c r="G60" s="119"/>
-      <c r="H60" s="119"/>
-      <c r="I60" s="119" t="s">
+      <c r="F61" s="118"/>
+      <c r="G61" s="118"/>
+      <c r="H61" s="118"/>
+      <c r="I61" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="120" t="s">
+      <c r="J61" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="K60" s="104" t="s">
+      <c r="K61" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="L60" s="104" t="s">
+      <c r="L61" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="M60" s="104">
+      <c r="M61" s="103">
         <v>2</v>
       </c>
-      <c r="N60" s="120"/>
-      <c r="O60" s="104" t="s">
+      <c r="N61" s="119"/>
+      <c r="O61" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="P60" s="104" t="s">
+      <c r="P61" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="Q60" s="104">
+      <c r="Q61" s="103">
         <v>6</v>
       </c>
-      <c r="R60" s="120"/>
-      <c r="S60" s="138"/>
-      <c r="T60" s="132"/>
-      <c r="U60" s="121"/>
-    </row>
-    <row r="61" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
-      <c r="B61" s="131" t="s">
+      <c r="R61" s="119"/>
+      <c r="S61" s="137"/>
+      <c r="T61" s="131"/>
+      <c r="U61" s="120"/>
+    </row>
+    <row r="62" spans="2:29" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B62" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="100">
+      <c r="C62" s="99">
         <v>1</v>
       </c>
-      <c r="D61" s="139">
+      <c r="D62" s="138">
         <v>0.5</v>
       </c>
-      <c r="E61" s="118">
+      <c r="E62" s="117">
         <v>1</v>
       </c>
-      <c r="F61" s="119"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="119" t="s">
+      <c r="F62" s="118"/>
+      <c r="G62" s="118"/>
+      <c r="H62" s="118"/>
+      <c r="I62" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="J61" s="120"/>
-      <c r="K61" s="120"/>
-      <c r="L61" s="120"/>
-      <c r="M61" s="120"/>
-      <c r="N61" s="120"/>
-      <c r="O61" s="120"/>
-      <c r="P61" s="120"/>
-      <c r="Q61" s="120"/>
-      <c r="R61" s="120"/>
-      <c r="S61" s="120"/>
-      <c r="T61" s="132"/>
-      <c r="U61" s="121"/>
-    </row>
-    <row r="62" spans="2:29" s="3" customFormat="1" ht="9" customHeight="1">
-      <c r="B62" s="140"/>
-      <c r="C62" s="141"/>
-      <c r="D62" s="142"/>
-      <c r="E62" s="143"/>
-      <c r="F62" s="144"/>
-      <c r="G62" s="144"/>
-      <c r="H62" s="144"/>
-      <c r="I62" s="144"/>
-      <c r="J62" s="145"/>
-      <c r="K62" s="145"/>
-      <c r="L62" s="145"/>
-      <c r="M62" s="145"/>
-      <c r="N62" s="145"/>
-      <c r="O62" s="145"/>
-      <c r="P62" s="145"/>
-      <c r="Q62" s="145"/>
-      <c r="R62" s="145"/>
-      <c r="S62" s="145"/>
-      <c r="T62" s="145"/>
-      <c r="U62" s="146"/>
+      <c r="J62" s="119"/>
+      <c r="K62" s="119"/>
+      <c r="L62" s="119"/>
+      <c r="M62" s="119"/>
+      <c r="N62" s="119"/>
+      <c r="O62" s="119"/>
+      <c r="P62" s="119"/>
+      <c r="Q62" s="119"/>
+      <c r="R62" s="119"/>
+      <c r="S62" s="119"/>
+      <c r="T62" s="131"/>
+      <c r="U62" s="120"/>
+    </row>
+    <row r="63" spans="2:29" s="3" customFormat="1" ht="9" customHeight="1">
+      <c r="B63" s="139"/>
+      <c r="C63" s="140"/>
+      <c r="D63" s="141"/>
+      <c r="E63" s="142"/>
+      <c r="F63" s="143"/>
+      <c r="G63" s="143"/>
+      <c r="H63" s="143"/>
+      <c r="I63" s="143"/>
+      <c r="J63" s="144"/>
+      <c r="K63" s="144"/>
+      <c r="L63" s="144"/>
+      <c r="M63" s="144"/>
+      <c r="N63" s="144"/>
+      <c r="O63" s="144"/>
+      <c r="P63" s="144"/>
+      <c r="Q63" s="144"/>
+      <c r="R63" s="144"/>
+      <c r="S63" s="144"/>
+      <c r="T63" s="144"/>
+      <c r="U63" s="145"/>
+    </row>
+    <row r="64" spans="2:29" s="1" customFormat="1" ht="16" customHeight="1">
+      <c r="B64" s="113" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" s="128"/>
+      <c r="D64" s="128"/>
+      <c r="E64" s="128"/>
+      <c r="F64" s="128"/>
+      <c r="G64" s="128"/>
+      <c r="H64" s="128"/>
+      <c r="I64" s="128"/>
+      <c r="J64" s="128"/>
+      <c r="K64" s="128"/>
+      <c r="L64" s="128"/>
+      <c r="M64" s="128"/>
+      <c r="N64" s="128"/>
+      <c r="O64" s="128"/>
+      <c r="P64" s="128"/>
+      <c r="Q64" s="128"/>
+      <c r="R64" s="128"/>
+      <c r="S64" s="128"/>
+      <c r="T64" s="128"/>
+      <c r="U64" s="129"/>
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3"/>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3"/>
+      <c r="AC64" s="3"/>
+    </row>
+    <row r="65" spans="2:21" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B65" s="130" t="s">
+        <v>223</v>
+      </c>
+      <c r="C65" s="99">
+        <v>1</v>
+      </c>
+      <c r="D65" s="117">
+        <v>1</v>
+      </c>
+      <c r="E65" s="117">
+        <v>3</v>
+      </c>
+      <c r="F65" s="118"/>
+      <c r="G65" s="118"/>
+      <c r="H65" s="118"/>
+      <c r="I65" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65" s="119"/>
+      <c r="K65" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="L65" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="M65" s="119">
+        <v>2</v>
+      </c>
+      <c r="N65" s="119"/>
+      <c r="O65" s="119" t="s">
+        <v>64</v>
+      </c>
+      <c r="P65" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" s="119">
+        <v>14</v>
+      </c>
+      <c r="R65" s="119"/>
+      <c r="S65" s="119" t="s">
+        <v>229</v>
+      </c>
+      <c r="T65" s="131" t="s">
+        <v>231</v>
+      </c>
+      <c r="U65" s="120">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="2:21" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B66" s="132" t="s">
+        <v>224</v>
+      </c>
+      <c r="C66" s="133">
+        <v>1</v>
+      </c>
+      <c r="D66" s="134">
+        <v>1</v>
+      </c>
+      <c r="E66" s="101">
+        <v>9</v>
+      </c>
+      <c r="F66" s="135"/>
+      <c r="G66" s="135"/>
+      <c r="H66" s="135"/>
+      <c r="I66" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="L66" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="M66" s="103">
+        <v>2</v>
+      </c>
+      <c r="N66" s="103"/>
+      <c r="O66" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="P66" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66" s="103">
+        <v>6</v>
+      </c>
+      <c r="R66" s="103"/>
+      <c r="S66" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="T66" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="U66" s="104">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="2:21" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B67" s="130" t="s">
+        <v>225</v>
+      </c>
+      <c r="C67" s="133">
+        <v>1</v>
+      </c>
+      <c r="D67" s="134">
+        <v>1.5</v>
+      </c>
+      <c r="E67" s="101">
+        <v>2</v>
+      </c>
+      <c r="F67" s="135"/>
+      <c r="G67" s="135"/>
+      <c r="H67" s="135"/>
+      <c r="I67" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="K67" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="L67" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="M67" s="103">
+        <v>2</v>
+      </c>
+      <c r="N67" s="103"/>
+      <c r="O67" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="P67" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q67" s="103">
+        <v>6</v>
+      </c>
+      <c r="R67" s="103"/>
+      <c r="S67" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T67" s="103" t="s">
+        <v>231</v>
+      </c>
+      <c r="U67" s="104">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:21" s="3" customFormat="1" ht="22" customHeight="1">
+      <c r="B68" s="132" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" s="133">
+        <v>1</v>
+      </c>
+      <c r="D68" s="134">
+        <v>2</v>
+      </c>
+      <c r="E68" s="101">
+        <v>2</v>
+      </c>
+      <c r="F68" s="135"/>
+      <c r="G68" s="135"/>
+      <c r="H68" s="135"/>
+      <c r="I68" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="K68" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="L68" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="M68" s="103">
+        <v>2</v>
+      </c>
+      <c r="N68" s="103"/>
+      <c r="O68" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="P68" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q68" s="103">
+        <v>6</v>
+      </c>
+      <c r="R68" s="103"/>
+      <c r="S68" s="103"/>
+      <c r="T68" s="103"/>
+      <c r="U68" s="104"/>
+    </row>
+    <row r="69" spans="2:21" s="3" customFormat="1" ht="9" customHeight="1">
+      <c r="B69" s="139"/>
+      <c r="C69" s="140"/>
+      <c r="D69" s="141"/>
+      <c r="E69" s="142"/>
+      <c r="F69" s="143"/>
+      <c r="G69" s="143"/>
+      <c r="H69" s="143"/>
+      <c r="I69" s="143"/>
+      <c r="J69" s="144"/>
+      <c r="K69" s="144"/>
+      <c r="L69" s="144"/>
+      <c r="M69" s="144"/>
+      <c r="N69" s="144"/>
+      <c r="O69" s="144"/>
+      <c r="P69" s="144"/>
+      <c r="Q69" s="144"/>
+      <c r="R69" s="144"/>
+      <c r="S69" s="144"/>
+      <c r="T69" s="144"/>
+      <c r="U69" s="145"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="B3:U3"/>
     <mergeCell ref="B27:U27"/>
     <mergeCell ref="B35:U35"/>
+    <mergeCell ref="B64:U64"/>
     <mergeCell ref="B18:U18"/>
     <mergeCell ref="B8:U8"/>
     <mergeCell ref="B1:U1"/>
-    <mergeCell ref="B52:U52"/>
+    <mergeCell ref="B53:U53"/>
     <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B46:U46"/>
+    <mergeCell ref="B47:U47"/>
     <mergeCell ref="J41:U41"/>
     <mergeCell ref="B22:U22"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K48 O48 S50 S48 O50" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K49 O49 S51 S49 O51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F53:I61 F50:I50 F47:I48" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F54:I62 F51:I51 F48:I49 F65:I68" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>DataSource</formula1>
     </dataValidation>
   </dataValidations>
@@ -4412,8 +4747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -4540,8 +4875,12 @@
         <v>61</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="13"/>
+      <c r="H5" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>230</v>
+      </c>
       <c r="K5" s="4" t="s">
         <v>42</v>
       </c>
@@ -4564,9 +4903,15 @@
         <v>63</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
@@ -4576,9 +4921,15 @@
       <c r="C7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="19" t="s">
@@ -4590,9 +4941,15 @@
       <c r="C8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
@@ -4606,17 +4963,23 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
@@ -6145,7 +6508,12 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5fb5e84a-5684-468e-b345-7aeeb4845130">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c891a41a-a233-45b7-a3f1-ec06333a8c94" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -6159,8 +6527,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f83516c0962013713c7b05e4bc5e59d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="752b74123ce8ce04e6dc2ca32a236890" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aaf53faa0b720e0e3b2b5121d0fe8108">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88a8651ba02bfcc8abd053d50e01d782" ns2:_="" ns3:_="">
     <xsd:import namespace="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
     <xsd:import namespace="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
     <xsd:element name="properties">
@@ -6182,6 +6550,8 @@
                 <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6217,6 +6587,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ae301ee1-5209-4650-b0c1-2c09e3e2885c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="c891a41a-a233-45b7-a3f1-ec06333a8c94">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5fb5e84a-5684-468e-b345-7aeeb4845130" elementFormDefault="qualified">
@@ -6280,6 +6661,13 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="bdf4d8d7-af3c-42ab-a689-3e7dc994f6b2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -6407,20 +6795,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44D8FFA3-65C9-43F9-8D4E-F7555189104B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
-    <ds:schemaRef ds:uri="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43999CC8-E95C-400B-9A7C-F3AE8E0025CB}"/>
 </file>
</xml_diff>